<commit_message>
guardando cambios antes de mover a rama ronald
</commit_message>
<xml_diff>
--- a/Basededatos/FQOLTC.xlsx
+++ b/Basededatos/FQOLTC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20417"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://luzdelsurlds-my.sharepoint.com/personal/roquispec_luzdelsur_com_pe/Documents/Documentos/Estudios de Ingreso/ProyectoRyD_V2/Basededatos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_AD4D2F04E46CFB4ACB3E20031514F388693EDF25" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36B32C19-2562-41BB-9893-6F67334BDBF2}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="113_{FDD29332-0684-4F45-98D9-C5FA50E9BE52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{B2844730-78B0-41C2-9248-613B04F06A45}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -433,7 +433,7 @@
   <dimension ref="B2:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D3" sqref="D3:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,12 +465,8 @@
       <c r="C3" s="2">
         <v>44693</v>
       </c>
-      <c r="D3" s="4">
-        <v>18</v>
-      </c>
-      <c r="E3" s="4">
-        <v>48</v>
-      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
@@ -479,12 +475,8 @@
       <c r="C4" s="2">
         <v>43232</v>
       </c>
-      <c r="D4" s="4">
-        <v>33</v>
-      </c>
-      <c r="E4" s="4">
-        <v>12</v>
-      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
@@ -493,12 +485,8 @@
       <c r="C5" s="2">
         <v>42734</v>
       </c>
-      <c r="D5" s="4">
-        <v>34</v>
-      </c>
-      <c r="E5" s="4">
-        <v>14</v>
-      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
@@ -507,12 +495,8 @@
       <c r="C6" s="2">
         <v>41724</v>
       </c>
-      <c r="D6" s="4">
-        <v>48</v>
-      </c>
-      <c r="E6" s="4">
-        <v>46</v>
-      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -521,12 +505,8 @@
       <c r="C7" s="2">
         <v>44730</v>
       </c>
-      <c r="D7" s="4">
-        <v>58</v>
-      </c>
-      <c r="E7" s="4">
-        <v>33</v>
-      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -535,12 +515,8 @@
       <c r="C8" s="2">
         <v>43108</v>
       </c>
-      <c r="D8" s="4">
-        <v>36</v>
-      </c>
-      <c r="E8" s="4">
-        <v>10</v>
-      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -549,12 +525,8 @@
       <c r="C9" s="2">
         <v>42904</v>
       </c>
-      <c r="D9" s="4">
-        <v>47</v>
-      </c>
-      <c r="E9" s="4">
-        <v>48</v>
-      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
@@ -563,12 +535,8 @@
       <c r="C10" s="2">
         <v>42443</v>
       </c>
-      <c r="D10" s="4">
-        <v>18</v>
-      </c>
-      <c r="E10" s="4">
-        <v>59</v>
-      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
@@ -577,12 +545,8 @@
       <c r="C11" s="2">
         <v>45489</v>
       </c>
-      <c r="D11" s="4">
-        <v>28</v>
-      </c>
-      <c r="E11" s="4">
-        <v>19</v>
-      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
@@ -591,12 +555,8 @@
       <c r="C12" s="2">
         <v>42815</v>
       </c>
-      <c r="D12" s="4">
-        <v>33</v>
-      </c>
-      <c r="E12" s="4">
-        <v>13</v>
-      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
@@ -605,12 +565,8 @@
       <c r="C13" s="2">
         <v>41994</v>
       </c>
-      <c r="D13" s="4">
-        <v>57</v>
-      </c>
-      <c r="E13" s="4">
-        <v>17</v>
-      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
@@ -619,12 +575,8 @@
       <c r="C14" s="2">
         <v>41635</v>
       </c>
-      <c r="D14" s="4">
-        <v>33</v>
-      </c>
-      <c r="E14" s="4">
-        <v>32</v>
-      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
@@ -633,12 +585,8 @@
       <c r="C15" s="2">
         <v>45609</v>
       </c>
-      <c r="D15" s="4">
-        <v>50</v>
-      </c>
-      <c r="E15" s="4">
-        <v>57</v>
-      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
@@ -647,12 +595,8 @@
       <c r="C16" s="2">
         <v>43407</v>
       </c>
-      <c r="D16" s="4">
-        <v>43</v>
-      </c>
-      <c r="E16" s="4">
-        <v>26</v>
-      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
@@ -661,12 +605,8 @@
       <c r="C17" s="2">
         <v>42909</v>
       </c>
-      <c r="D17" s="4">
-        <v>35</v>
-      </c>
-      <c r="E17" s="4">
-        <v>20</v>
-      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
@@ -675,12 +615,8 @@
       <c r="C18" s="2">
         <v>42531</v>
       </c>
-      <c r="D18" s="4">
-        <v>39</v>
-      </c>
-      <c r="E18" s="4">
-        <v>29</v>
-      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>